<commit_message>
CARLA-2 DD and DPE for CARLA
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
@@ -1,22 +1,188 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>valueType</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>tg</t>
+  </si>
+  <si>
+    <t>chol</t>
+  </si>
+  <si>
+    <t>ldlc</t>
+  </si>
+  <si>
+    <t>hdl</t>
+  </si>
+  <si>
+    <t>bmi</t>
+  </si>
+  <si>
+    <t>f1_bmi</t>
+  </si>
+  <si>
+    <t>f1_taillenumfang</t>
+  </si>
+  <si>
+    <t>taillenumfang</t>
+  </si>
+  <si>
+    <t>hueftumfang</t>
+  </si>
+  <si>
+    <t>f1_hueftumfang</t>
+  </si>
+  <si>
+    <t>f1_age</t>
+  </si>
+  <si>
+    <t>Triglyceride (mmol/l)</t>
+  </si>
+  <si>
+    <t>Cholesterol (mmol/l)</t>
+  </si>
+  <si>
+    <t>LDL measured (mmol/l)</t>
+  </si>
+  <si>
+    <t>HDL (mmol/l)</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Age at follow-up</t>
+  </si>
+  <si>
+    <t>gj</t>
+  </si>
+  <si>
+    <t>total energy intake at baseline</t>
+  </si>
+  <si>
+    <t>zk</t>
+  </si>
+  <si>
+    <t>total carbohydrates at baseline</t>
+  </si>
+  <si>
+    <t>ze</t>
+  </si>
+  <si>
+    <t>total protein intake at baseline</t>
+  </si>
+  <si>
+    <t>zf</t>
+  </si>
+  <si>
+    <t>total fat intake at baseline</t>
+  </si>
+  <si>
+    <t>za</t>
+  </si>
+  <si>
+    <t>total alcohol intake at baseline</t>
+  </si>
+  <si>
+    <t>zb</t>
+  </si>
+  <si>
+    <t>dietary fiber intake at baseline</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>total saturated fatty acids intake at baseline</t>
+  </si>
+  <si>
+    <t>fu</t>
+  </si>
+  <si>
+    <t>total monounsaturated fatty acids intake at baseline</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>total polyunsaturated fatty acids intake at baseline</t>
+  </si>
+  <si>
+    <t>kd</t>
+  </si>
+  <si>
+    <t>total daily dissaccharides intake at baseline</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>total daily monosaccharides intake at baseline</t>
+  </si>
+  <si>
+    <t>kmt</t>
+  </si>
+  <si>
+    <t>glucose</t>
+  </si>
+  <si>
+    <t>kmf</t>
+  </si>
+  <si>
+    <t>fructose</t>
+  </si>
+  <si>
+    <t>mna</t>
+  </si>
+  <si>
+    <t>natrium</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>kalium</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,6 +197,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,22 +245,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -110,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +365,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +400,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,63 +576,341 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>valueType</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CARLA Corrected version from Iness
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC6F61D-3017-40AD-8A92-BB6AC30EC511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -88,100 +89,100 @@
     <t>Age at follow-up</t>
   </si>
   <si>
-    <t>gj</t>
-  </si>
-  <si>
-    <t>total energy intake at baseline</t>
-  </si>
-  <si>
-    <t>zk</t>
-  </si>
-  <si>
-    <t>total carbohydrates at baseline</t>
-  </si>
-  <si>
-    <t>ze</t>
-  </si>
-  <si>
-    <t>total protein intake at baseline</t>
-  </si>
-  <si>
-    <t>zf</t>
-  </si>
-  <si>
-    <t>total fat intake at baseline</t>
-  </si>
-  <si>
-    <t>za</t>
-  </si>
-  <si>
-    <t>total alcohol intake at baseline</t>
-  </si>
-  <si>
-    <t>zb</t>
-  </si>
-  <si>
-    <t>dietary fiber intake at baseline</t>
-  </si>
-  <si>
-    <t>fs</t>
-  </si>
-  <si>
-    <t>total saturated fatty acids intake at baseline</t>
-  </si>
-  <si>
-    <t>fu</t>
-  </si>
-  <si>
-    <t>total monounsaturated fatty acids intake at baseline</t>
-  </si>
-  <si>
-    <t>fp</t>
-  </si>
-  <si>
-    <t>total polyunsaturated fatty acids intake at baseline</t>
-  </si>
-  <si>
-    <t>kd</t>
-  </si>
-  <si>
-    <t>total daily dissaccharides intake at baseline</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>total daily monosaccharides intake at baseline</t>
-  </si>
-  <si>
-    <t>kmt</t>
-  </si>
-  <si>
-    <t>glucose</t>
-  </si>
-  <si>
-    <t>kmf</t>
-  </si>
-  <si>
-    <t>fructose</t>
-  </si>
-  <si>
-    <t>mna</t>
-  </si>
-  <si>
-    <t>natrium</t>
-  </si>
-  <si>
-    <t>mk</t>
-  </si>
-  <si>
-    <t>kalium</t>
+    <t>GJ</t>
+  </si>
+  <si>
+    <t>Gesamtenergie [kJ/Tag]</t>
+  </si>
+  <si>
+    <t>Kohlenhydrate [g/Tag]</t>
+  </si>
+  <si>
+    <t>ZK</t>
+  </si>
+  <si>
+    <t>Eiweiß [g/Tag]</t>
+  </si>
+  <si>
+    <t>ZE</t>
+  </si>
+  <si>
+    <t>Fett [g/Tag]</t>
+  </si>
+  <si>
+    <t>ZF</t>
+  </si>
+  <si>
+    <t>Alkohol [g/Tag]</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>Ballaststoffe [g/Tag]</t>
+  </si>
+  <si>
+    <t>ZB</t>
+  </si>
+  <si>
+    <t>gesättigte Fettsäuren [g/Tag]</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>einfach ungesättigte Fettsaeuren [g/Tag]</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>mehrfach ungesättigte Fettsaeuren [g/Tag]</t>
+  </si>
+  <si>
+    <t>Disaccharide [g/Tag]</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>Monosaccharide [g/Tag]</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>Glucose [g/Tag]</t>
+  </si>
+  <si>
+    <t>KMT</t>
+  </si>
+  <si>
+    <t>Fructose [g/Tag]</t>
+  </si>
+  <si>
+    <t>KMF</t>
+  </si>
+  <si>
+    <t>Natrium [g/Tag]</t>
+  </si>
+  <si>
+    <t>MNA</t>
+  </si>
+  <si>
+    <t>Kalium [g/Tag]</t>
+  </si>
+  <si>
+    <t>MK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,14 +214,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -245,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,9 +261,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -275,7 +271,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -291,7 +287,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -366,6 +362,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -401,6 +414,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,19 +606,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
@@ -613,7 +643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -624,7 +654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -635,7 +665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -646,7 +676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -657,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -668,7 +698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -679,7 +709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -690,7 +720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -701,7 +731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -712,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -723,168 +753,168 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D18" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D21" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="8" t="s">
+      <c r="D23" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="D24" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
+      <c r="D25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="10" t="s">
+      <c r="D26" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -895,14 +925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Z19: I dont why this changed because I didnt not touch her algorith on my local drive. but I have checked and 4.184 is the correct one. Z28: semicolon placed between variables. No spacing. Z36: mna indicated.
All variable are in lower cases.
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC6F61D-3017-40AD-8A92-BB6AC30EC511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B57ED01-96CC-4D53-91B7-FA72A1561684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,94 +89,94 @@
     <t>Age at follow-up</t>
   </si>
   <si>
-    <t>GJ</t>
-  </si>
-  <si>
     <t>Gesamtenergie [kJ/Tag]</t>
   </si>
   <si>
     <t>Kohlenhydrate [g/Tag]</t>
   </si>
   <si>
-    <t>ZK</t>
-  </si>
-  <si>
     <t>Eiweiß [g/Tag]</t>
   </si>
   <si>
-    <t>ZE</t>
-  </si>
-  <si>
     <t>Fett [g/Tag]</t>
   </si>
   <si>
-    <t>ZF</t>
-  </si>
-  <si>
     <t>Alkohol [g/Tag]</t>
   </si>
   <si>
-    <t>ZA</t>
-  </si>
-  <si>
     <t>Ballaststoffe [g/Tag]</t>
   </si>
   <si>
-    <t>ZB</t>
-  </si>
-  <si>
-    <t>gesättigte Fettsäuren [g/Tag]</t>
-  </si>
-  <si>
-    <t>FS</t>
-  </si>
-  <si>
-    <t>einfach ungesättigte Fettsaeuren [g/Tag]</t>
-  </si>
-  <si>
-    <t>FU</t>
-  </si>
-  <si>
-    <t>FP</t>
-  </si>
-  <si>
-    <t>mehrfach ungesättigte Fettsaeuren [g/Tag]</t>
-  </si>
-  <si>
     <t>Disaccharide [g/Tag]</t>
   </si>
   <si>
-    <t>KD</t>
-  </si>
-  <si>
     <t>Monosaccharide [g/Tag]</t>
   </si>
   <si>
-    <t>KM</t>
-  </si>
-  <si>
     <t>Glucose [g/Tag]</t>
   </si>
   <si>
-    <t>KMT</t>
-  </si>
-  <si>
     <t>Fructose [g/Tag]</t>
   </si>
   <si>
-    <t>KMF</t>
-  </si>
-  <si>
     <t>Natrium [g/Tag]</t>
   </si>
   <si>
-    <t>MNA</t>
-  </si>
-  <si>
     <t>Kalium [g/Tag]</t>
   </si>
   <si>
-    <t>MK</t>
+    <t>gj</t>
+  </si>
+  <si>
+    <t>zk</t>
+  </si>
+  <si>
+    <t>ze</t>
+  </si>
+  <si>
+    <t>zf</t>
+  </si>
+  <si>
+    <t>za</t>
+  </si>
+  <si>
+    <t>zb</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>fu</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>kd</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>kmt</t>
+  </si>
+  <si>
+    <t>kmf</t>
+  </si>
+  <si>
+    <t>mna</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>Gesättigte Fettsäuren [g/Tag]</t>
+  </si>
+  <si>
+    <t>Einfach ungesättigte Fettsaeuren [g/Tag]</t>
+  </si>
+  <si>
+    <t>Mehrfach ungesättigte Fettsaeuren [g/Tag]</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +755,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>20</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>20</v>
@@ -777,10 +777,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>20</v>
@@ -788,10 +788,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>20</v>
@@ -799,10 +799,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>20</v>
@@ -810,10 +810,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>20</v>
@@ -821,10 +821,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>20</v>
@@ -832,10 +832,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>20</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>20</v>
@@ -854,10 +854,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>20</v>
@@ -865,10 +865,10 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>20</v>
@@ -879,7 +879,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>20</v>
@@ -887,10 +887,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>20</v>
@@ -898,10 +898,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>20</v>
@@ -909,10 +909,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
CARLA-3 Files after branch fix
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_CARLA_INES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B57ED01-96CC-4D53-91B7-FA72A1561684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3528F21-AD7C-4423-9D45-041FADA26AAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>